<commit_message>
Update rfq responded products template
</commit_message>
<xml_diff>
--- a/src/private/templates/rfq_responded_products.xlsx
+++ b/src/private/templates/rfq_responded_products.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>suggestedManufacturer</t>
   </si>
@@ -45,6 +45,27 @@
   </si>
   <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>purchaseRequestNumber</t>
+  </si>
+  <si>
+    <t>shortText</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>uom</t>
+  </si>
+  <si>
+    <t>manufacturer</t>
+  </si>
+  <si>
+    <t>manufacturerPartNumber</t>
   </si>
 </sst>
 </file>
@@ -359,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="244" zoomScaleNormal="244" zoomScalePageLayoutView="244" workbookViewId="0"/>
   </sheetViews>
@@ -372,26 +393,47 @@
     <col min="7" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="I1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="L1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="N1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added awardNote, awardAttachments fields
</commit_message>
<xml_diff>
--- a/src/private/templates/rfq_responded_products.xlsx
+++ b/src/private/templates/rfq_responded_products.xlsx
@@ -433,7 +433,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="108" zoomScaleNormal="108" zoomScalePageLayoutView="108" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,13 +499,16 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048576">
       <formula1>"DDP - OT UB warehouse, DDP - OT site, FCA - Supplier Facility, EXW"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N1048576">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576">
+      <formula1>"MNT,USD"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>